<commit_message>
Se sube Modelo adaptado y funcional
</commit_message>
<xml_diff>
--- a/Parametros_unicos.xlsx
+++ b/Parametros_unicos.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB17A02E-D56D-43F6-9AE1-6EDD74F117CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matiasorbetafranco/gurobi-tareas/gurobi-vitacura/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87DBAC8-5A5A-F148-BC53-FBDC9B39DD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,7 +57,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,15 +412,16 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -431,7 +437,7 @@
         <v>97388</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -439,7 +445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -447,12 +453,12 @@
         <v>39780</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>723248</v>
+        <v>723248000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>